<commit_message>
update readme, input settings, cooling schedules, add requriments.txt
</commit_message>
<xml_diff>
--- a/data/generated_data/best_solution/timetables/group_0.xlsx
+++ b/data/generated_data/best_solution/timetables/group_0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>Hours</t>
   </si>
@@ -73,82 +73,85 @@
     <t>{}</t>
   </si>
   <si>
-    <t>{0: sala nr 4 | Piotr Wójcik | Biologia}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 9 | Karolina Kamińska | Chemia}</t>
+    <t>{0: sala nr 4 | Paweł Lewandowski | Matematyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 10 | Natalia Szymańska | Geografia}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 10 | Zofia Wiśniewska | Wychowanie fizyczne}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 8 | Paweł Lewandowski | Matematyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 1 | Jan Nowak | Język polski}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 6 | Jan Nowak | Język polski}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 11 | Paweł Lewandowski | Matematyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 5 | Karolina Kamińska | Chemia}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 4 | Mateusz Kowalski | Język niemiecki}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 8 | Katarzyna Mazur | Fizyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 2 | Natalia Szymańska | Geografia}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 4 | Dominik Kaczor | Informatyka}</t>
   </si>
   <si>
     <t>{0: sala nr 3 | Dominik Kaczor | Informatyka}</t>
   </si>
   <si>
-    <t>{0: sala nr 1 | Lena Kowalska | Język angielski}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 9 | Dominik Kaczor | Informatyka}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 4 | Zofia Wiśniewska | Wychowanie fizyczne}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 11 | Piotr Wójcik | Biologia}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 9 | Katarzyna Mazur | Fizyka}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 9 | Paweł Lewandowski | Matematyka}</t>
+    <t>{0: sala nr 7 | Dominik Kaczor | Informatyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 8 | Lena Kowalska | Język angielski}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 2 | Mateusz Kowalski | Język niemiecki}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 7 | Karolina Kamińska | Chemia}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 11 | Katarzyna Mazur | Fizyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 11 | Lena Kowalska | Język angielski}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 3 | Piotr Wójcik | Biologia}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 3 | Paweł Lewandowski | Matematyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 10 | Katarzyna Mazur | Fizyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 9 | Piotr Wójcik | Biologia}</t>
   </si>
   <si>
     <t>{0: sala nr 1 | Dominik Kaczor | Informatyka}</t>
   </si>
   <si>
-    <t>{0: sala nr 5 | Lena Kowalska | Język angielski}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 8 | Karolina Kamińska | Chemia}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 1 | Paweł Lewandowski | Matematyka}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 1 | Jan Nowak | Język polski}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 5 | Paweł Lewandowski | Matematyka}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 3 | Mateusz Kowalski | Język niemiecki}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 4 | Paweł Lewandowski | Matematyka}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 2 | Lena Kowalska | Język angielski}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 7 | Zofia Wiśniewska | Wychowanie fizyczne}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 10 | Mateusz Kowalski | Język niemiecki}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 11 | Natalia Szymańska | Geografia}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 6 | Jan Nowak | Język polski}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 1 | Katarzyna Mazur | Fizyka}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 10 | Dominik Kaczor | Informatyka}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 8 | Natalia Szymańska | Geografia}</t>
-  </si>
-  <si>
-    <t>{0: sala nr 9 | Zofia Wiśniewska | Wychowanie fizyczne}</t>
+    <t>{0: sala nr 8 | Jan Nowak | Język polski}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 7 | Paweł Lewandowski | Matematyka}</t>
+  </si>
+  <si>
+    <t>{0: sala nr 3 | Zofia Wiśniewska | Wychowanie fizyczne}</t>
   </si>
 </sst>
 </file>
@@ -513,10 +516,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" customWidth="1"/>
     <col min="4" max="4" width="51.7109375" customWidth="1"/>
-    <col min="5" max="5" width="55.7109375" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" customWidth="1"/>
     <col min="6" max="6" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -548,13 +551,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -568,16 +571,16 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -588,16 +591,16 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -605,19 +608,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -625,19 +628,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -645,19 +648,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -665,19 +668,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -685,7 +688,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -694,10 +697,10 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -705,10 +708,10 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -717,7 +720,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -728,7 +731,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -737,7 +740,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -748,16 +751,16 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -768,16 +771,16 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>